<commit_message>
added coment in plan
</commit_message>
<xml_diff>
--- a/План работ.xlsx
+++ b/План работ.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10911"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11008"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/work/Desktop/Project/Sergey_Tinkoff_Bot/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/arg/Desktop/Project_M1/Sergey_Tinkoff_Bot/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F457918D-8269-AE43-924C-1ABA372C6C42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A10B9BC2-AB9F-FF46-A2F7-9639B2BB5AC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" xr2:uid="{A2E45735-841D-AF45-BDE4-D6AF469921B6}"/>
+    <workbookView xWindow="360" yWindow="760" windowWidth="25480" windowHeight="17160" xr2:uid="{A2E45735-841D-AF45-BDE4-D6AF469921B6}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
         <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
@@ -151,7 +150,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -176,6 +175,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -189,7 +194,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -217,6 +222,12 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -536,7 +547,7 @@
   <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="159" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -581,32 +592,32 @@
     </row>
     <row r="4" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2"/>
-      <c r="B4" s="5">
+      <c r="B4" s="11">
         <v>1</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="D4" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="E4" s="12" t="s">
         <v>24</v>
       </c>
       <c r="F4" s="2"/>
     </row>
     <row r="5" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="2"/>
-      <c r="B5" s="9">
+      <c r="B5" s="11">
         <v>2</v>
       </c>
-      <c r="C5" s="10" t="s">
+      <c r="C5" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="9" t="s">
+      <c r="D5" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="E5" s="10" t="s">
+      <c r="E5" s="12" t="s">
         <v>25</v>
       </c>
       <c r="F5" s="2"/>

</xml_diff>